<commit_message>
Add task 2 (BT2)
</commit_message>
<xml_diff>
--- a/BT1_DFS_BFS_UCS_for_Sokoban/Bao_cao/Ket_qua.xlsx
+++ b/BT1_DFS_BFS_UCS_for_Sokoban/Bao_cao/Ket_qua.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_File\UIT\CS106_TTNT_AI\BT1_DFS_BFS_UCS_for_Sokoban\Bao_cao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A98EE9-8CBC-4821-9316-A85A3ADB7A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CA7E86-D1EA-4CB3-83D0-76E4A78B74D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1011,7 +1011,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B2" sqref="B2:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>